<commit_message>
feat(.gitignore): updated gitingore file to remove cache, csvs and models directory
</commit_message>
<xml_diff>
--- a/model_summary.xlsx
+++ b/model_summary.xlsx
@@ -1,20 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/goharshoukat/Documents/GitHub/synthetic-CPT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBAD8762-BA1C-664D-A3F7-2C0ACD4F4AF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F157F8E4-829C-4243-8D34-ED71C4AF9845}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17240" activeTab="1" xr2:uid="{E3E7E9B6-9E30-6B40-9D65-5577E9355D32}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17240" activeTab="10" xr2:uid="{E3E7E9B6-9E30-6B40-9D65-5577E9355D32}"/>
   </bookViews>
   <sheets>
     <sheet name="First Second" sheetId="1" r:id="rId1"/>
     <sheet name="Third" sheetId="2" r:id="rId2"/>
+    <sheet name="Fourth" sheetId="3" r:id="rId3"/>
+    <sheet name="Fifth" sheetId="4" r:id="rId4"/>
+    <sheet name="Sixth" sheetId="5" r:id="rId5"/>
+    <sheet name="Seventh" sheetId="6" r:id="rId6"/>
+    <sheet name="Eigth" sheetId="7" r:id="rId7"/>
+    <sheet name="EigthV2" sheetId="8" r:id="rId8"/>
+    <sheet name="Ninth" sheetId="9" r:id="rId9"/>
+    <sheet name="Eleventh" sheetId="10" r:id="rId10"/>
+    <sheet name="Twelveth" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="76">
   <si>
     <t>Hidden Layers</t>
   </si>
@@ -287,6 +296,87 @@
   </si>
   <si>
     <t>4 times</t>
+  </si>
+  <si>
+    <t>Summary</t>
+  </si>
+  <si>
+    <t>Test data shows poor performance</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>L1L2(l1=1e-6, l2=1e-6)</t>
+  </si>
+  <si>
+    <t>L2(1e-6)</t>
+  </si>
+  <si>
+    <t>L1L2(l1=1e-7, l2=1e-7)</t>
+  </si>
+  <si>
+    <t>L2(1e-7)</t>
+  </si>
+  <si>
+    <t>Inputs</t>
+  </si>
+  <si>
+    <t>Lat</t>
+  </si>
+  <si>
+    <t>lng</t>
+  </si>
+  <si>
+    <t>bathymetry</t>
+  </si>
+  <si>
+    <t>depth</t>
+  </si>
+  <si>
+    <t>lat, lng, bathy, depth</t>
+  </si>
+  <si>
+    <t>L1(1e-6)</t>
+  </si>
+  <si>
+    <t>0, 1, 3, 5, 7</t>
+  </si>
+  <si>
+    <t>L1</t>
+  </si>
+  <si>
+    <t>L2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ridge regression: applied to all features. </t>
+  </si>
+  <si>
+    <t>Lasso regression: shrinks the less important features, inbuilt feature selection</t>
+  </si>
+  <si>
+    <t>weright regularizer</t>
+  </si>
+  <si>
+    <t>activity regularizer / output</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data used for this model is filtered using univariate cubic spline with mostly a smoothing parameter of 0.5 for all cases except 10 and 11. For these two, 0.1 was used. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data used is unfiltered one. </t>
+  </si>
+  <si>
+    <t>edge points deeted for the wrong cpt profiles, doesn’t include ﻿['CPT_03.csv', 'CPT_05.csv', 'CPT_05a.csv', 'CPT_06.csv', 'CPT_08.csv'] due to gas sublayers</t>
+  </si>
+  <si>
+    <t>CPT 9 and 11 also reomved due to poor consistency</t>
+  </si>
+  <si>
+    <t>L1L2(l1=1e-5, l2=1e-5)</t>
+  </si>
+  <si>
+    <t>L1(1e-5)</t>
   </si>
 </sst>
 </file>
@@ -367,7 +457,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -387,6 +477,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -702,10 +795,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E8D849B-E90D-D34E-A96A-3CCFFDDB3EB6}">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:M20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F1"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -713,7 +806,7 @@
     <col min="4" max="4" width="62.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:13">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -734,7 +827,7 @@
       </c>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:13">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -754,7 +847,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:13">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -774,7 +867,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:13">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -794,7 +887,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:13">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -814,7 +907,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:13">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -834,7 +927,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:13">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -854,7 +947,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:13">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -874,7 +967,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:13">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -894,30 +987,83 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="14" spans="1:13">
+      <c r="L14" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="M14" s="4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="32">
       <c r="A15" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="16" spans="1:7">
+      <c r="L15" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="M15" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="32">
       <c r="A16" t="s">
         <v>20</v>
       </c>
       <c r="B16" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="17" spans="1:1">
+      <c r="L16" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="M16" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="33">
       <c r="A17" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="18" spans="1:1">
+      <c r="L17" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="M17" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13">
       <c r="A18" t="s">
         <v>25</v>
+      </c>
+      <c r="L18" s="3"/>
+      <c r="M18" s="3"/>
+    </row>
+    <row r="19" spans="1:13">
+      <c r="L19" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="M19" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13">
+      <c r="A20" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20" t="s">
+        <v>57</v>
+      </c>
+      <c r="C20" t="s">
+        <v>58</v>
+      </c>
+      <c r="D20" t="s">
+        <v>59</v>
+      </c>
+      <c r="E20" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -925,12 +1071,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19B70B60-E19A-5B46-847E-973A8CF7C56A}">
-  <dimension ref="A1:S12"/>
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFEE8F45-53E9-3F4F-80AF-5420631311F3}">
+  <dimension ref="A1:S24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1004,19 +1150,19 @@
         <v>29</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>48</v>
+        <v>63</v>
+      </c>
+      <c r="G2" s="3">
+        <v>5</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>32</v>
+        <v>74</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>33</v>
+        <v>75</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>34</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:19">
@@ -1036,19 +1182,19 @@
         <v>41</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>30</v>
+        <v>63</v>
       </c>
       <c r="G3" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>32</v>
+        <v>74</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>33</v>
+        <v>75</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>34</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:19">
@@ -1068,19 +1214,19 @@
         <v>42</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>30</v>
+        <v>63</v>
       </c>
       <c r="G4" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>32</v>
+        <v>74</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>33</v>
+        <v>75</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>34</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:19">
@@ -1100,19 +1246,19 @@
         <v>43</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>30</v>
+        <v>63</v>
       </c>
       <c r="G5" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>32</v>
+        <v>74</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>33</v>
+        <v>75</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>34</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:19" ht="33">
@@ -1132,19 +1278,19 @@
         <v>403</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>30</v>
+        <v>63</v>
       </c>
       <c r="G6" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>32</v>
+        <v>74</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>33</v>
+        <v>75</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>34</v>
+        <v>75</v>
       </c>
       <c r="S6" s="5" t="s">
         <v>37</v>
@@ -1159,6 +1305,650 @@
       </c>
     </row>
     <row r="10" spans="1:19" ht="32">
+      <c r="A10" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="O10" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="P10" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" ht="32">
+      <c r="A11" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="O11" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="P11" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" ht="33">
+      <c r="A12" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="O12" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="P12" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19">
+      <c r="O14" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="P14" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19">
+      <c r="O15" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="P15" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="24" spans="9:9">
+      <c r="I24" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A10:I10"/>
+    <mergeCell ref="A11:I11"/>
+    <mergeCell ref="A12:J12"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90532538-2B98-CB4A-B5BE-66ACF7E6E121}">
+  <dimension ref="A1:S24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="7.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="12.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.83203125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="19.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="14" width="10.83203125" style="3"/>
+    <col min="15" max="15" width="16.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="108.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20.83203125" style="3" customWidth="1"/>
+    <col min="18" max="18" width="10.83203125" style="3"/>
+    <col min="19" max="19" width="12.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="10.83203125" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="P1" s="4"/>
+    </row>
+    <row r="2" spans="1:19">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" s="3">
+        <v>9</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="3">
+        <v>1</v>
+      </c>
+      <c r="G2" s="3">
+        <v>5</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="3">
+        <v>7</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F3" s="3">
+        <v>1</v>
+      </c>
+      <c r="G3" s="3">
+        <v>4</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" s="3">
+        <v>5</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" s="3">
+        <v>1</v>
+      </c>
+      <c r="G4" s="3">
+        <v>3</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19">
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" s="3">
+        <v>3</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="F5" s="3">
+        <v>1</v>
+      </c>
+      <c r="G5" s="3">
+        <v>2</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" ht="33">
+      <c r="A6" s="3">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6" s="3">
+        <v>1</v>
+      </c>
+      <c r="E6" s="7">
+        <v>403</v>
+      </c>
+      <c r="F6" s="3">
+        <v>1</v>
+      </c>
+      <c r="G6" s="3">
+        <v>1</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="S6" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19">
+      <c r="O9" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="P9" s="4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" ht="32">
+      <c r="A10" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="O10" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="P10" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" ht="32">
+      <c r="A11" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="O11" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="P11" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" ht="33">
+      <c r="A12" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="O12" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="P12" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19">
+      <c r="O14" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="P14" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19">
+      <c r="O15" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="P15" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="24" spans="9:9">
+      <c r="I24" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A10:I10"/>
+    <mergeCell ref="A11:I11"/>
+    <mergeCell ref="A12:J12"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19B70B60-E19A-5B46-847E-973A8CF7C56A}">
+  <dimension ref="A1:S24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="7.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="12.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.83203125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="19.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="14" width="10.83203125" style="3"/>
+    <col min="15" max="15" width="16.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="108.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20.83203125" style="3" customWidth="1"/>
+    <col min="18" max="18" width="10.83203125" style="3"/>
+    <col min="19" max="19" width="12.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="10.83203125" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="P1" s="4"/>
+    </row>
+    <row r="2" spans="1:19">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" s="3">
+        <v>9</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="3">
+        <v>7</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3" s="3">
+        <v>3</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" s="3">
+        <v>5</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4" s="3">
+        <v>2</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19">
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" s="3">
+        <v>3</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" s="3">
+        <v>1</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" ht="33">
+      <c r="A6" s="3">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6" s="3">
+        <v>1</v>
+      </c>
+      <c r="E6" s="7">
+        <v>403</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" s="3">
+        <v>0</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="S6" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19">
+      <c r="O9" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="P9" s="4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" ht="32">
       <c r="O10" s="3" t="s">
         <v>36</v>
       </c>
@@ -1180,10 +1970,2143 @@
       </c>
       <c r="P12" s="3" t="s">
         <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19">
+      <c r="O14" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="P14" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="9:16">
+      <c r="O17" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="P17" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="24" spans="9:16">
+      <c r="I24" s="3" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99250388-C7CD-8C47-AE78-CFC8EC40AA0C}">
+  <dimension ref="A1:S24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="7.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="12.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.83203125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="19.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="14" width="10.83203125" style="3"/>
+    <col min="15" max="15" width="16.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="108.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20.83203125" style="3" customWidth="1"/>
+    <col min="18" max="18" width="10.83203125" style="3"/>
+    <col min="19" max="19" width="12.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="10.83203125" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="P1" s="4"/>
+    </row>
+    <row r="2" spans="1:19">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" s="3">
+        <v>9</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G2" s="3">
+        <v>5</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="3">
+        <v>7</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G3" s="3">
+        <v>4</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" s="3">
+        <v>5</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G4" s="3">
+        <v>3</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19">
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" s="3">
+        <v>3</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G5" s="3">
+        <v>2</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" ht="33">
+      <c r="A6" s="3">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6" s="3">
+        <v>1</v>
+      </c>
+      <c r="E6" s="7">
+        <v>403</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G6" s="3">
+        <v>1</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="S6" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19">
+      <c r="O9" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="P9" s="4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" ht="32">
+      <c r="O10" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="P10" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" ht="32">
+      <c r="O11" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="P11" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" ht="33">
+      <c r="O12" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="P12" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19">
+      <c r="O14" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="P14" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19">
+      <c r="O15" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="P15" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="24" spans="9:9">
+      <c r="I24" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C752159-463A-6746-B7BC-AE74878C1054}">
+  <dimension ref="A1:S24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="7.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="12.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.83203125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="19.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="14" width="10.83203125" style="3"/>
+    <col min="15" max="15" width="16.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="108.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20.83203125" style="3" customWidth="1"/>
+    <col min="18" max="18" width="10.83203125" style="3"/>
+    <col min="19" max="19" width="12.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="10.83203125" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="P1" s="4"/>
+    </row>
+    <row r="2" spans="1:19">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" s="3">
+        <v>9</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G2" s="3">
+        <v>5</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="3">
+        <v>7</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G3" s="3">
+        <v>4</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" s="3">
+        <v>5</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G4" s="3">
+        <v>3</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19">
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" s="3">
+        <v>3</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G5" s="3">
+        <v>2</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" ht="33">
+      <c r="A6" s="3">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6" s="3">
+        <v>1</v>
+      </c>
+      <c r="E6" s="7">
+        <v>403</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G6" s="3">
+        <v>1</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="S6" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19">
+      <c r="O9" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="P9" s="4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" ht="32">
+      <c r="O10" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="P10" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" ht="32">
+      <c r="O11" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="P11" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" ht="33">
+      <c r="O12" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="P12" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19">
+      <c r="O14" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="P14" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19">
+      <c r="O15" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="P15" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="9:16">
+      <c r="O18" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="P18" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="19" spans="9:16">
+      <c r="O19" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="P19" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="24" spans="9:16">
+      <c r="I24" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{590B2B11-2F6C-5646-9BE2-5D2E2FA4A1F4}">
+  <dimension ref="A1:S24"/>
+  <sheetViews>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="J26" sqref="J26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="7.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="12.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.83203125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="19.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="14" width="10.83203125" style="3"/>
+    <col min="15" max="15" width="16.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="108.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20.83203125" style="3" customWidth="1"/>
+    <col min="18" max="18" width="10.83203125" style="3"/>
+    <col min="19" max="19" width="12.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="10.83203125" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="P1" s="4"/>
+    </row>
+    <row r="2" spans="1:19">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" s="3">
+        <v>9</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G2" s="3">
+        <v>5</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="3">
+        <v>7</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G3" s="3">
+        <v>4</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" s="3">
+        <v>5</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G4" s="3">
+        <v>3</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19">
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" s="3">
+        <v>3</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G5" s="3">
+        <v>2</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" ht="33">
+      <c r="A6" s="3">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6" s="3">
+        <v>1</v>
+      </c>
+      <c r="E6" s="7">
+        <v>403</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G6" s="3">
+        <v>1</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="S6" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19">
+      <c r="O9" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="P9" s="4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" ht="32">
+      <c r="O10" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="P10" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" ht="32">
+      <c r="O11" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="P11" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" ht="33">
+      <c r="O12" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="P12" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19">
+      <c r="O14" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="P14" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19">
+      <c r="O15" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="P15" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="24" spans="9:9">
+      <c r="I24" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCBF7B2B-AB46-3C46-86F9-9EC684184E4B}">
+  <dimension ref="A1:S24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="7.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="12.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.83203125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="19.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="14" width="10.83203125" style="3"/>
+    <col min="15" max="15" width="16.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="108.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20.83203125" style="3" customWidth="1"/>
+    <col min="18" max="18" width="10.83203125" style="3"/>
+    <col min="19" max="19" width="12.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="10.83203125" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="P1" s="4"/>
+    </row>
+    <row r="2" spans="1:19">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" s="3">
+        <v>9</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G2" s="3">
+        <v>5</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="3">
+        <v>7</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G3" s="3">
+        <v>4</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" s="3">
+        <v>5</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G4" s="3">
+        <v>3</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19">
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" s="3">
+        <v>3</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G5" s="3">
+        <v>2</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" ht="33">
+      <c r="A6" s="3">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6" s="3">
+        <v>1</v>
+      </c>
+      <c r="E6" s="7">
+        <v>403</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G6" s="3">
+        <v>1</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="S6" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19">
+      <c r="O9" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="P9" s="4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" ht="32">
+      <c r="A10" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="O10" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="P10" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" ht="32">
+      <c r="O11" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="P11" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" ht="33">
+      <c r="O12" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="P12" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19">
+      <c r="O14" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="P14" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19">
+      <c r="O15" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="P15" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="24" spans="9:9">
+      <c r="I24" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A10:I10"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA2F3A2A-A2F6-E34E-9AF7-BA1BA42E3C41}">
+  <dimension ref="A1:S24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:I11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="7.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="12.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.83203125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="19.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="14" width="10.83203125" style="3"/>
+    <col min="15" max="15" width="16.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="108.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20.83203125" style="3" customWidth="1"/>
+    <col min="18" max="18" width="10.83203125" style="3"/>
+    <col min="19" max="19" width="12.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="10.83203125" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="P1" s="4"/>
+    </row>
+    <row r="2" spans="1:19">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" s="3">
+        <v>9</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G2" s="3">
+        <v>5</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="3">
+        <v>7</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G3" s="3">
+        <v>4</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" s="3">
+        <v>5</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G4" s="3">
+        <v>3</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19">
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" s="3">
+        <v>3</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G5" s="3">
+        <v>2</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" ht="33">
+      <c r="A6" s="3">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6" s="3">
+        <v>1</v>
+      </c>
+      <c r="E6" s="7">
+        <v>403</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G6" s="3">
+        <v>1</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S6" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19">
+      <c r="O9" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="P9" s="4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" ht="32">
+      <c r="A10" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="O10" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="P10" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" ht="32">
+      <c r="A11" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="O11" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="P11" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" ht="33">
+      <c r="A12" s="8"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="O12" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="P12" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19">
+      <c r="O14" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="P14" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19">
+      <c r="O15" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="P15" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="24" spans="9:9">
+      <c r="I24" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A10:I10"/>
+    <mergeCell ref="A11:I11"/>
+    <mergeCell ref="A12:I12"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{413D64B2-1866-E64B-BD9A-8A186043E756}">
+  <dimension ref="A1:S24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O8" sqref="O8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="7.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="12.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.83203125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="19.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="14" width="10.83203125" style="3"/>
+    <col min="15" max="15" width="16.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="108.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20.83203125" style="3" customWidth="1"/>
+    <col min="18" max="18" width="10.83203125" style="3"/>
+    <col min="19" max="19" width="12.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="10.83203125" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="P1" s="4"/>
+    </row>
+    <row r="2" spans="1:19">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" s="3">
+        <v>9</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G2" s="3">
+        <v>5</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="3">
+        <v>7</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G3" s="3">
+        <v>4</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" s="3">
+        <v>5</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G4" s="3">
+        <v>3</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19">
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" s="3">
+        <v>3</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G5" s="3">
+        <v>2</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" ht="33">
+      <c r="A6" s="3">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6" s="3">
+        <v>1</v>
+      </c>
+      <c r="E6" s="7">
+        <v>403</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G6" s="3">
+        <v>1</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="S6" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19">
+      <c r="O9" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="P9" s="4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" ht="32">
+      <c r="A10" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="O10" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="P10" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" ht="32">
+      <c r="A11" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="O11" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="P11" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" ht="33">
+      <c r="O12" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="P12" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19">
+      <c r="O14" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="P14" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19">
+      <c r="O15" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="P15" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="24" spans="9:9">
+      <c r="I24" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A10:I10"/>
+    <mergeCell ref="A11:I11"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1156BFF-B6ED-F64D-AD6E-A264F42C8C5A}">
+  <dimension ref="A1:S24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:I10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="7.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="12.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.83203125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="19.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="14" width="10.83203125" style="3"/>
+    <col min="15" max="15" width="16.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="108.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20.83203125" style="3" customWidth="1"/>
+    <col min="18" max="18" width="10.83203125" style="3"/>
+    <col min="19" max="19" width="12.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="10.83203125" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="P1" s="4"/>
+    </row>
+    <row r="2" spans="1:19">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" s="3">
+        <v>9</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G2" s="3">
+        <v>5</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="3">
+        <v>7</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G3" s="3">
+        <v>4</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" s="3">
+        <v>5</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G4" s="3">
+        <v>3</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19">
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" s="3">
+        <v>3</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G5" s="3">
+        <v>2</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" ht="33">
+      <c r="A6" s="3">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6" s="3">
+        <v>1</v>
+      </c>
+      <c r="E6" s="7">
+        <v>403</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G6" s="3">
+        <v>1</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="S6" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19">
+      <c r="O9" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="P9" s="4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" ht="32">
+      <c r="A10" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="O10" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="P10" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" ht="32">
+      <c r="A11" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="O11" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="P11" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" ht="33">
+      <c r="A12" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="O12" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="P12" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19">
+      <c r="O14" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="P14" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19">
+      <c r="O15" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="P15" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="24" spans="9:9">
+      <c r="I24" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A10:I10"/>
+    <mergeCell ref="A11:I11"/>
+    <mergeCell ref="A12:J12"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>